<commit_message>
Added top and bottom layout picture for the DDS and update deliverable review
</commit_message>
<xml_diff>
--- a/Douglas/Deliverables Review.xlsx
+++ b/Douglas/Deliverables Review.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27430"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2140" yWindow="460" windowWidth="24480" windowHeight="16340" tabRatio="500"/>
+    <workbookView xWindow="4280" yWindow="0" windowWidth="24480" windowHeight="16340" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" calcOnSave="0" concurrentCalc="0"/>
+  <calcPr calcId="140000" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="74">
   <si>
     <t>Author</t>
   </si>
@@ -168,6 +168,99 @@
       </rPr>
       <t>Why a half second? That seems like a really long time for a microcontroller</t>
     </r>
+  </si>
+  <si>
+    <t>Realization</t>
+  </si>
+  <si>
+    <t>Schematic</t>
+  </si>
+  <si>
+    <t>No Title</t>
+  </si>
+  <si>
+    <t>No Revision</t>
+  </si>
+  <si>
+    <t>No Designer</t>
+  </si>
+  <si>
+    <t>No standard part call  out (R and C)</t>
+  </si>
+  <si>
+    <t>Good Organization</t>
+  </si>
+  <si>
+    <t>Add color label to LED1</t>
+  </si>
+  <si>
+    <t>Ardu_to_Tiny_Mainsignal is not descriptive</t>
+  </si>
+  <si>
+    <t>Make your net names descriptive. For example for the Ard_Sig_Header_XXX signals. What is the difference between them? Then use that to name the net</t>
+  </si>
+  <si>
+    <t>POT is not doing anything. Match the circuit from the wepage</t>
+  </si>
+  <si>
+    <t>Add Decoupling cap to VCC for the ATTINY</t>
+  </si>
+  <si>
+    <t>All ICs and Connectors should have part numbers displayed</t>
+  </si>
+  <si>
+    <t>Minor siganls, such as DCC_RC do not have to be displayed. Is there a way to do that in Altium?</t>
+  </si>
+  <si>
+    <t>Move references that are overlapping the edge of the board so they are not cut off (e.g. HDR4)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resistor packages look like 0603. They should be 1206. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Since the headers going into the sheild are soldered to the bottom side of the board they will block soldering. </t>
+  </si>
+  <si>
+    <t>Move all traces that intersect these pads to the Top side of the board</t>
+  </si>
+  <si>
+    <t>The speaker pads look too small to solder to. Most of the pads is covered by the speaker</t>
+  </si>
+  <si>
+    <t>Make the pads into larger rectangles</t>
+  </si>
+  <si>
+    <t>The LED component outline indicates a right angle LED. Is that accurate? If not update the outline to match the actual package</t>
+  </si>
+  <si>
+    <t>Align Pot2 with Pot_5k and the LED. Make the user interface logical and easiy to understand</t>
+  </si>
+  <si>
+    <t>Make sure the board matches the design rules.i.e. 30° v bit for the traces and 1/32 end mill for the board outline and holes</t>
+  </si>
+  <si>
+    <t>Layout</t>
+  </si>
+  <si>
+    <t>Adjust placement so the traces flow logically and are easy to route</t>
+  </si>
+  <si>
+    <t>R2 and C3 are hard to distinguish</t>
+  </si>
+  <si>
+    <t>Push button switch does not have pull up or pull down resistor</t>
+  </si>
+  <si>
+    <t>Decide what logic you want and add a resistor in the appropriate position</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Can R2,C3,C1,C2 be connected directly to the gound plane without needing a trace? The connection could be made a lot lower resistance than it is now. </t>
+  </si>
+  <si>
+    <t>Center speaker placement. There is now need to make the board bigger in that dimension</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Placement seems random. </t>
   </si>
 </sst>
 </file>
@@ -254,7 +347,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -268,8 +361,28 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -293,20 +406,41 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="33">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -636,17 +770,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="49" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="49.83203125" style="6" customWidth="1"/>
     <col min="5" max="5" width="41.5" style="6" customWidth="1"/>
     <col min="6" max="6" width="37.6640625" style="6" customWidth="1"/>
   </cols>
@@ -984,6 +1118,359 @@
       </c>
       <c r="D22" s="8" t="s">
         <v>42</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26">
+        <v>0.1</v>
+      </c>
+      <c r="B26" t="s">
+        <v>1</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27">
+        <v>0.1</v>
+      </c>
+      <c r="B27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28">
+        <v>0.1</v>
+      </c>
+      <c r="B28" t="s">
+        <v>1</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29">
+        <v>0.1</v>
+      </c>
+      <c r="B29" t="s">
+        <v>1</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30">
+        <v>0.1</v>
+      </c>
+      <c r="B30" t="s">
+        <v>1</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31">
+        <v>0.1</v>
+      </c>
+      <c r="B31" t="s">
+        <v>1</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32">
+        <v>0.1</v>
+      </c>
+      <c r="B32" t="s">
+        <v>1</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33">
+        <v>0.1</v>
+      </c>
+      <c r="B33" t="s">
+        <v>1</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="45">
+      <c r="A34">
+        <v>0.1</v>
+      </c>
+      <c r="B34" t="s">
+        <v>1</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="30">
+      <c r="A35">
+        <v>0.1</v>
+      </c>
+      <c r="B35" t="s">
+        <v>1</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="30">
+      <c r="A36">
+        <v>0.1</v>
+      </c>
+      <c r="B36" t="s">
+        <v>1</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37">
+        <v>0.1</v>
+      </c>
+      <c r="B37" t="s">
+        <v>1</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="30">
+      <c r="A38">
+        <v>0.1</v>
+      </c>
+      <c r="B38" t="s">
+        <v>1</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="30">
+      <c r="A39">
+        <v>0.1</v>
+      </c>
+      <c r="B39" t="s">
+        <v>1</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E39" s="7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="30">
+      <c r="A40">
+        <v>0.1</v>
+      </c>
+      <c r="B40" t="s">
+        <v>1</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41">
+        <v>0.1</v>
+      </c>
+      <c r="B41" t="s">
+        <v>1</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="30">
+      <c r="A42">
+        <v>0.1</v>
+      </c>
+      <c r="B42" t="s">
+        <v>1</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E42" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="30">
+      <c r="A43">
+        <v>0.1</v>
+      </c>
+      <c r="B43" t="s">
+        <v>1</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E43" s="6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="45">
+      <c r="A44">
+        <v>0.1</v>
+      </c>
+      <c r="B44" t="s">
+        <v>1</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="30">
+      <c r="A45">
+        <v>0.1</v>
+      </c>
+      <c r="B45" t="s">
+        <v>1</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="45">
+      <c r="A46">
+        <v>0.1</v>
+      </c>
+      <c r="B46" t="s">
+        <v>1</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D46" s="7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47">
+        <v>0.1</v>
+      </c>
+      <c r="B47" t="s">
+        <v>1</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="45">
+      <c r="A48">
+        <v>0.1</v>
+      </c>
+      <c r="B48" t="s">
+        <v>1</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="30">
+      <c r="A49">
+        <v>0.1</v>
+      </c>
+      <c r="B49" t="s">
+        <v>1</v>
+      </c>
+      <c r="C49" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>